<commit_message>
- Fix layout add new user - Add function: send email after created a user
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F07-MinhTran\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vacation\VacationTracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,12 +17,11 @@
     <sheet name="Mobile" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="72">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -194,6 +193,8 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
       </rPr>
       <t xml:space="preserve"> if he/she is active state and then employee can't login into system
 - Able to </t>
@@ -213,6 +214,8 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
       </rPr>
       <t xml:space="preserve"> employee account</t>
     </r>
@@ -236,32 +239,10 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> by input the email</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">- Able to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
       </rPr>
-      <t>create new account</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> with some information: first name, last name, position, gender, phone number, email,...
-- Able to send email to employee with password default after creating</t>
+      <t xml:space="preserve"> by input the email</t>
     </r>
   </si>
   <si>
@@ -349,6 +330,8 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
       </rPr>
       <t xml:space="preserve">
 - Able to </t>
@@ -366,6 +349,8 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
       </rPr>
       <t xml:space="preserve">
 - Able to </t>
@@ -385,6 +370,8 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
       </rPr>
       <t xml:space="preserve"> employees
 - Able to see some </t>
@@ -404,6 +391,8 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
       </rPr>
       <t xml:space="preserve"> such as: </t>
     </r>
@@ -422,6 +411,8 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
       </rPr>
       <t xml:space="preserve">, edit, </t>
     </r>
@@ -440,6 +431,8 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -453,6 +446,231 @@
         <charset val="163"/>
       </rPr>
       <t>view detail</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>create new account</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> with some information: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>first name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>last name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>position,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>gender,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>phone number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">,…
+- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>send email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> to employee </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>with password default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> after creating</t>
+    </r>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>login</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>email and password</t>
     </r>
   </si>
 </sst>
@@ -470,45 +688,63 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <b/>
       <u/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="10"/>
@@ -601,7 +837,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -722,9 +958,6 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -742,9 +975,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -766,6 +996,20 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1274,7 +1518,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1306,9 +1550,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="34"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -1342,14 +1586,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -1359,18 +1603,20 @@
       <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="60"/>
+      <c r="B4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="52" t="s">
-        <v>11</v>
+      <c r="D4" s="62"/>
+      <c r="E4" s="64" t="s">
+        <v>71</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="63" t="s">
+        <v>70</v>
+      </c>
       <c r="G4" s="15"/>
       <c r="H4" s="7"/>
       <c r="I4" s="16"/>
@@ -1380,14 +1626,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -1397,18 +1643,20 @@
       <c r="M5" s="16"/>
     </row>
     <row r="6" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="37"/>
+      <c r="B6" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="36" t="s">
-        <v>46</v>
+      <c r="D6" s="40"/>
+      <c r="E6" s="59" t="s">
+        <v>69</v>
       </c>
-      <c r="F6" s="33"/>
+      <c r="F6" s="59" t="s">
+        <v>70</v>
+      </c>
       <c r="G6" s="15"/>
       <c r="H6" s="7"/>
       <c r="I6" s="16"/>
@@ -1426,8 +1674,8 @@
         <v>18</v>
       </c>
       <c r="D7" s="24"/>
-      <c r="E7" s="36" t="s">
-        <v>69</v>
+      <c r="E7" s="33" t="s">
+        <v>68</v>
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="15"/>
@@ -1501,7 +1749,7 @@
       <c r="L10" s="16"/>
       <c r="M10" s="16"/>
     </row>
-    <row r="11" spans="1:13" s="47" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="46" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="37"/>
       <c r="B11" s="38" t="s">
         <v>9</v>
@@ -1513,26 +1761,26 @@
       <c r="E11" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="42" t="s">
-        <v>57</v>
+      <c r="F11" s="39" t="s">
+        <v>70</v>
       </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
       <c r="G12" s="15"/>
       <c r="H12" s="7"/>
       <c r="I12" s="16"/>
@@ -1572,7 +1820,7 @@
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="15"/>
@@ -1584,14 +1832,14 @@
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
       <c r="G15" s="15"/>
       <c r="H15" s="7"/>
       <c r="I15" s="16"/>
@@ -1605,7 +1853,7 @@
       <c r="B16" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="51" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="24"/>
@@ -1613,7 +1861,7 @@
         <v>43</v>
       </c>
       <c r="F16" s="32"/>
-      <c r="G16" s="54" t="s">
+      <c r="G16" s="52" t="s">
         <v>26</v>
       </c>
       <c r="H16" s="7"/>
@@ -1680,14 +1928,14 @@
       <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="56"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -15310,126 +15558,126 @@
   <cols>
     <col min="1" max="1" width="9.140625" style="31"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="50"/>
+    <col min="3" max="3" width="9.140625" style="49"/>
     <col min="5" max="5" width="56.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="50"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="48"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="50" t="s">
-        <v>57</v>
+      <c r="C3" s="49" t="s">
+        <v>56</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E3" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="48"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="48"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="49"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>48</v>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>54</v>
       </c>
-      <c r="C3" s="50" t="s">
-        <v>57</v>
+      <c r="C7" s="49" t="s">
+        <v>56</v>
       </c>
-      <c r="E3" s="51" t="s">
-        <v>59</v>
+      <c r="E7" s="50" t="s">
+        <v>63</v>
       </c>
-      <c r="G3" s="49"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>49</v>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E8" s="50" t="s">
+        <v>64</v>
       </c>
-      <c r="C4" s="50" t="s">
-        <v>57</v>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E9" s="48" t="s">
+        <v>65</v>
       </c>
-      <c r="E4" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="49"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="49" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="51" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="51" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E8" s="51" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E9" s="49" t="s">
+      <c r="E10" s="50" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="C11" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="50" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="50" t="s">
-        <v>57</v>
+      <c r="C12" s="49" t="s">
+        <v>56</v>
       </c>
-      <c r="E11" s="51" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="50" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="48" t="s">
-        <v>56</v>
+      <c r="B14" s="47" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -15478,9 +15726,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -15514,14 +15762,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -15552,14 +15800,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -15590,14 +15838,14 @@
       <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
       <c r="G7" s="15"/>
       <c r="H7" s="7"/>
       <c r="I7" s="16"/>

</xml_diff>

<commit_message>
- Fix something in user_detail - Change view template
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vacation\VacationTracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Company\Futurify\Project\Vacation\VacationTracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
     <sheet name="Mobile" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -673,6 +673,10 @@
       <t>email and password</t>
     </r>
   </si>
+  <si>
+    <t>fix something in viewdetail
+change view layout</t>
+  </si>
 </sst>
 </file>
 
@@ -981,6 +985,20 @@
     <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -996,20 +1014,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1518,7 +1522,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1528,7 +1532,7 @@
     <col min="3" max="3" width="54.28515625" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" customWidth="1"/>
     <col min="5" max="5" width="112.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="31" customWidth="1"/>
     <col min="7" max="9" width="25.85546875" customWidth="1"/>
     <col min="10" max="10" width="19.140625" customWidth="1"/>
     <col min="11" max="11" width="21.28515625" customWidth="1"/>
@@ -1550,9 +1554,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="34"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -1586,14 +1590,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -1603,18 +1607,18 @@
       <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="60"/>
+      <c r="A4" s="54"/>
       <c r="B4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="64" t="s">
+      <c r="D4" s="56"/>
+      <c r="E4" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="63" t="s">
+      <c r="F4" s="57" t="s">
         <v>70</v>
       </c>
       <c r="G4" s="15"/>
@@ -1626,14 +1630,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -1651,10 +1655,10 @@
         <v>14</v>
       </c>
       <c r="D6" s="40"/>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="53" t="s">
         <v>70</v>
       </c>
       <c r="G6" s="15"/>
@@ -1677,7 +1681,9 @@
       <c r="E7" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="32"/>
+      <c r="F7" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="G7" s="15"/>
       <c r="H7" s="7"/>
       <c r="I7" s="16"/>
@@ -1773,14 +1779,14 @@
       <c r="M11" s="44"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
       <c r="G12" s="15"/>
       <c r="H12" s="7"/>
       <c r="I12" s="16"/>
@@ -1832,14 +1838,14 @@
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
       <c r="G15" s="15"/>
       <c r="H15" s="7"/>
       <c r="I15" s="16"/>
@@ -1928,14 +1934,14 @@
       <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="54"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -15726,9 +15732,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -15762,14 +15768,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -15800,14 +15806,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -15838,14 +15844,14 @@
       <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
       <c r="G7" s="15"/>
       <c r="H7" s="7"/>
       <c r="I7" s="16"/>

</xml_diff>

<commit_message>
- Add error user login is inactive - Update user
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Company\Futurify\Project\Vacation\VacationTracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vacation\VacationTracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
     <sheet name="Mobile" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -174,54 +174,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">- Able to edit all general information: Name, DoB, Gender, Picture, Remaining days off...
-- Able to set employee to a deparment
-- Able to set employee to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>inactive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> if he/she is active state and then employee can't login into system
-- Able to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>reactivate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> employee account</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">'- Able to </t>
     </r>
     <r>
@@ -310,143 +262,6 @@
   </si>
   <si>
     <t>- Check token anywhere</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">- Able to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>see list of employees</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">
-- Able to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>search by keyword</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">
-- Able to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>filter or sort</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> employees
-- Able to see some </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>buttons</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> such as: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>add new</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">, edit, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>remove,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>view detail</t>
-    </r>
   </si>
   <si>
     <r>
@@ -674,8 +489,177 @@
     </r>
   </si>
   <si>
-    <t>fix something in viewdetail
-change view layout</t>
+    <t>Lỗi:</t>
+  </si>
+  <si>
+    <t>server trả về lỗi khi user/pass sai, làm sao để xóa bỏ</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Able to edit all general information: Name, DoB, Gender, Picture, Remaining days off...
+- Able to set employee to a deparment
+- Able to set employee to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>inactive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> if he/she is active state and then employee </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>can't login</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> into system
+- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>reactivate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> employee account</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>see list of employees</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">
+- Able to search by keyword
+- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>filter or sort</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> employees
+- Able to see some </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>buttons</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> such as: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>add new, edit, remove,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>view detail</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1522,7 +1506,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1616,10 +1600,10 @@
       </c>
       <c r="D4" s="56"/>
       <c r="E4" s="58" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F4" s="57" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="7"/>
@@ -1656,10 +1640,10 @@
       </c>
       <c r="D6" s="40"/>
       <c r="E6" s="53" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F6" s="53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="7"/>
@@ -1670,19 +1654,19 @@
       <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="37"/>
+      <c r="B7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="33" t="s">
+      <c r="D7" s="40"/>
+      <c r="E7" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="44" t="s">
         <v>68</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>72</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="7"/>
@@ -1722,8 +1706,8 @@
         <v>24</v>
       </c>
       <c r="D9" s="24"/>
-      <c r="E9" s="36" t="s">
-        <v>44</v>
+      <c r="E9" s="33" t="s">
+        <v>72</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="15"/>
@@ -1765,10 +1749,10 @@
       </c>
       <c r="D11" s="40"/>
       <c r="E11" s="41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G11" s="42"/>
       <c r="H11" s="43"/>
@@ -1826,7 +1810,7 @@
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="15"/>
@@ -15554,10 +15538,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15569,121 +15553,127 @@
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C1" s="49"/>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="48"/>
+      <c r="I2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="49" t="s">
-        <v>56</v>
+      <c r="C3" s="49" t="s">
+        <v>55</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E3" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="48"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="48"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="48"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>47</v>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>53</v>
       </c>
-      <c r="C3" s="49" t="s">
-        <v>56</v>
+      <c r="C7" s="49" t="s">
+        <v>55</v>
       </c>
-      <c r="E3" s="50" t="s">
-        <v>58</v>
+      <c r="E7" s="50" t="s">
+        <v>62</v>
       </c>
-      <c r="G3" s="48"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>48</v>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E8" s="50" t="s">
+        <v>63</v>
       </c>
-      <c r="C4" s="49" t="s">
-        <v>56</v>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E9" s="48" t="s">
+        <v>64</v>
       </c>
-      <c r="E4" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="48"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="48" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="50" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="50" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E8" s="50" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E9" s="48" t="s">
+      <c r="E10" s="50" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="C11" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="50" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="49" t="s">
-        <v>56</v>
+      <c r="C12" s="49" t="s">
+        <v>55</v>
       </c>
-      <c r="E11" s="50" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="49" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix some bugs: - Create new user must be active - Forget-password error, change to english (invalid token) - Confirm when delete account - Fix calculator vacation date - Reson field in vacation should be placeholder - Auto add 12 days for new user - Change remaining day to hours
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -13,15 +13,17 @@
   </bookViews>
   <sheets>
     <sheet name="Web" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="Mobile" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="87">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -134,10 +136,6 @@
     <t>As a admin, I want to manage all team in the system</t>
   </si>
   <si>
-    <t>- Able to cancel vacation that I booked
-- Team Lead and HR will recieve email notification</t>
-  </si>
-  <si>
     <t>Nice to have</t>
   </si>
   <si>
@@ -164,38 +162,6 @@
     <t>- Able to see list of day off on calendar that grouped by month
 - Able to filter by employee
 - Able to see the remaning day of employee</t>
-  </si>
-  <si>
-    <t>'- Each employee will have 12 days off (configurable), every time a vacation booked, employee's days off will be reduce accordingly
-- Able to book vacation with some information such as: from date - to date, from hour - to hour, reason
-- Able to see my vacation on google calendar
-- After submited, Team Lead and HR will recieve an email notification
-- Abe to edit submited vacation, Team Lead and HR will recieve email notification</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">'- Able to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>reset password</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> by input the email</t>
-    </r>
   </si>
   <si>
     <t>text Loi</t>
@@ -264,6 +230,54 @@
     <t>- Check token anywhere</t>
   </si>
   <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Lỗi:</t>
+  </si>
+  <si>
+    <t>server trả về lỗi khi user/pass sai, làm sao để xóa bỏ</t>
+  </si>
+  <si>
+    <t>From 9AM to 7PM</t>
+  </si>
+  <si>
+    <t>button inactive reverse, add status</t>
+  </si>
+  <si>
+    <t>remove old error when have new message</t>
+  </si>
+  <si>
+    <t>loading</t>
+  </si>
+  <si>
+    <t>defaut is active account</t>
+  </si>
+  <si>
+    <t>confirm when delete account</t>
+  </si>
+  <si>
+    <t>can't book when out of date</t>
+  </si>
+  <si>
+    <t>calculator date wrong</t>
+  </si>
+  <si>
+    <t>reason should be placeholder</t>
+  </si>
+  <si>
+    <t>auto add 12 days for new user</t>
+  </si>
+  <si>
+    <t>Thời hạn đổi mật khẩu đã hết (invalid token)</t>
+  </si>
+  <si>
+    <t>booking by day or hour</t>
+  </si>
+  <si>
+    <t>change remaing day to hours</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">- Able to </t>
     </r>
@@ -271,7 +285,43 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>login</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>email and password</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -281,17 +331,37 @@
     <r>
       <rPr>
         <sz val="10"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
       </rPr>
-      <t xml:space="preserve"> with some information: </t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>with some information:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -301,6 +371,7 @@
     <r>
       <rPr>
         <sz val="10"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -311,7 +382,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -321,6 +392,7 @@
     <r>
       <rPr>
         <sz val="10"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -331,7 +403,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -341,6 +413,7 @@
     <r>
       <rPr>
         <sz val="10"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -351,7 +424,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -361,6 +434,7 @@
     <r>
       <rPr>
         <sz val="10"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -371,7 +445,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -381,6 +455,7 @@
     <r>
       <rPr>
         <sz val="10"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -391,7 +466,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -412,7 +487,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -432,7 +507,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -442,19 +517,78 @@
     <r>
       <rPr>
         <sz val="10"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
       </rPr>
-      <t xml:space="preserve"> after creating</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>after creating</t>
     </r>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">- Able to </t>
+      <t>- Able to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>see list of employees</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">
+- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>search</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> by keyword
+- Able to </t>
     </r>
     <r>
       <rPr>
@@ -465,7 +599,7 @@
         <family val="2"/>
         <charset val="163"/>
       </rPr>
-      <t>login</t>
+      <t>filter</t>
     </r>
     <r>
       <rPr>
@@ -474,7 +608,7 @@
         <family val="2"/>
         <charset val="163"/>
       </rPr>
-      <t xml:space="preserve"> using </t>
+      <t xml:space="preserve"> or</t>
     </r>
     <r>
       <rPr>
@@ -485,14 +619,81 @@
         <family val="2"/>
         <charset val="163"/>
       </rPr>
-      <t>email and password</t>
+      <t xml:space="preserve"> </t>
     </r>
-  </si>
-  <si>
-    <t>Lỗi:</t>
-  </si>
-  <si>
-    <t>server trả về lỗi khi user/pass sai, làm sao để xóa bỏ</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>sort</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> employees
+- Able to see some </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>buttons</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> such as: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>add new, edit, remove,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>view detail</t>
+    </r>
   </si>
   <si>
     <r>
@@ -504,7 +705,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -524,7 +725,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -545,7 +746,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -564,18 +765,18 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">- Able to </t>
+      <t xml:space="preserve">'- Able to </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
       </rPr>
-      <t>see list of employees</t>
+      <t>reset password</t>
     </r>
     <r>
       <rPr>
@@ -584,65 +785,17 @@
         <family val="2"/>
         <charset val="163"/>
       </rPr>
-      <t xml:space="preserve">
-- Able to search by keyword
-- Able to </t>
+      <t xml:space="preserve"> by input the email</t>
     </r>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>filter or sort</t>
+      <t>- Able to</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> employees
-- Able to see some </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>buttons</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> such as: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>add new, edit, remove,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
@@ -653,12 +806,81 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B0F0"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="163"/>
       </rPr>
-      <t>view detail</t>
+      <t>cancel vacation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> that I booked
+- Team Lead and HR will recieve email notification</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>'- Each employee will have 12 days off (configurable), every time a vacation booked, employee's days off will be reduce accordingly
+- Able to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>book vacation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> with some information such as: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>from date - to date, from hour - to hour, reason</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">
+- Able to see my vacation on google calendar
+- After submited, Team Lead and HR will recieve an email notification
+- Abe to edit submited vacation, Team Lead and HR will recieve email notification</t>
     </r>
   </si>
 </sst>
@@ -666,7 +888,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -777,6 +999,27 @@
       <family val="2"/>
       <charset val="163"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -825,7 +1068,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -943,9 +1186,6 @@
     <xf numFmtId="4" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -999,6 +1239,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1506,15 +1748,15 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="54.28515625" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="112.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" style="31" customWidth="1"/>
     <col min="7" max="9" width="25.85546875" customWidth="1"/>
@@ -1538,9 +1780,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="34"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -1574,14 +1816,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -1591,19 +1833,19 @@
       <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="54"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="58" t="s">
-        <v>69</v>
+      <c r="D4" s="55"/>
+      <c r="E4" s="57" t="s">
+        <v>80</v>
       </c>
-      <c r="F4" s="57" t="s">
-        <v>68</v>
+      <c r="F4" s="56" t="s">
+        <v>64</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="7"/>
@@ -1614,14 +1856,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -1639,11 +1881,11 @@
         <v>14</v>
       </c>
       <c r="D6" s="40"/>
-      <c r="E6" s="53" t="s">
-        <v>67</v>
+      <c r="E6" s="52" t="s">
+        <v>81</v>
       </c>
-      <c r="F6" s="53" t="s">
-        <v>68</v>
+      <c r="F6" s="52" t="s">
+        <v>64</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="7"/>
@@ -1662,11 +1904,11 @@
         <v>18</v>
       </c>
       <c r="D7" s="40"/>
-      <c r="E7" s="53" t="s">
-        <v>73</v>
+      <c r="E7" s="52" t="s">
+        <v>82</v>
       </c>
-      <c r="F7" s="44" t="s">
-        <v>68</v>
+      <c r="F7" s="43" t="s">
+        <v>64</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="7"/>
@@ -1707,7 +1949,7 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="33" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="15"/>
@@ -1739,7 +1981,7 @@
       <c r="L10" s="16"/>
       <c r="M10" s="16"/>
     </row>
-    <row r="11" spans="1:13" s="46" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="45" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="37"/>
       <c r="B11" s="38" t="s">
         <v>9</v>
@@ -1748,29 +1990,29 @@
         <v>29</v>
       </c>
       <c r="D11" s="40"/>
-      <c r="E11" s="41" t="s">
-        <v>44</v>
+      <c r="E11" s="52" t="s">
+        <v>84</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
-      <c r="G11" s="42"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
       <c r="G12" s="15"/>
       <c r="H12" s="7"/>
       <c r="I12" s="16"/>
@@ -1810,7 +2052,7 @@
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="36" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="15"/>
@@ -1822,14 +2064,14 @@
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
       <c r="G15" s="15"/>
       <c r="H15" s="7"/>
       <c r="I15" s="16"/>
@@ -1843,15 +2085,17 @@
       <c r="B16" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="50" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="24"/>
-      <c r="E16" s="36" t="s">
-        <v>43</v>
+      <c r="E16" s="33" t="s">
+        <v>86</v>
       </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="52" t="s">
+      <c r="F16" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="51" t="s">
         <v>26</v>
       </c>
       <c r="H16" s="7"/>
@@ -1871,21 +2115,21 @@
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="33" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="F17" s="32"/>
     </row>
     <row r="18" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="23"/>
       <c r="B18" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="15"/>
@@ -1899,14 +2143,14 @@
     <row r="19" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="23"/>
       <c r="B19" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="15"/>
@@ -1918,14 +2162,14 @@
       <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="59" t="s">
-        <v>40</v>
+      <c r="A20" s="58" t="s">
+        <v>39</v>
       </c>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1940,11 +2184,11 @@
         <v>9</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="15" t="s">
@@ -15538,147 +15782,107 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="31"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="49"/>
-    <col min="5" max="5" width="56.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="49"/>
-      <c r="H1" s="31" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="64" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="64" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>45</v>
+    <row r="4" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="65" t="s">
+        <v>77</v>
       </c>
-      <c r="C2" s="49" t="s">
-        <v>55</v>
+      <c r="B4" s="64" t="s">
+        <v>52</v>
       </c>
-      <c r="E2" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="48"/>
-      <c r="I2" t="s">
+      <c r="C4" s="64"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="64" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>46</v>
+      <c r="B5" s="64" t="s">
+        <v>52</v>
       </c>
-      <c r="C3" s="49" t="s">
-        <v>55</v>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="64" t="s">
+        <v>72</v>
       </c>
-      <c r="E3" s="50" t="s">
-        <v>57</v>
+      <c r="B6" s="64" t="s">
+        <v>52</v>
       </c>
-      <c r="G3" s="48"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>47</v>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="64" t="s">
+        <v>73</v>
       </c>
-      <c r="C4" s="49" t="s">
-        <v>55</v>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="46" t="s">
+        <v>74</v>
       </c>
-      <c r="E4" s="50" t="s">
-        <v>58</v>
+      <c r="B8" s="64" t="s">
+        <v>52</v>
       </c>
-      <c r="F4" s="48" t="s">
-        <v>55</v>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="64" t="s">
+        <v>75</v>
       </c>
-      <c r="G4" s="48"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>48</v>
+      <c r="B9" s="64" t="s">
+        <v>52</v>
       </c>
-      <c r="C5" s="49" t="s">
-        <v>55</v>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="46" t="s">
+        <v>76</v>
       </c>
-      <c r="E5" s="48" t="s">
-        <v>59</v>
+      <c r="B10" s="64" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>49</v>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="64" t="s">
+        <v>78</v>
       </c>
-      <c r="C6" s="49" t="s">
-        <v>55</v>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="64" t="s">
+        <v>79</v>
       </c>
-      <c r="E6" s="50" t="s">
-        <v>61</v>
+      <c r="B12" s="64" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="50" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E8" s="50" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E9" s="48" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="50" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="50" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="47" t="s">
-        <v>54</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15722,9 +15926,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -15758,14 +15962,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -15796,14 +16000,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -15834,14 +16038,14 @@
       <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
       <c r="G7" s="15"/>
       <c r="H7" s="7"/>
       <c r="I7" s="16"/>
@@ -29482,4 +29686,150 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="31"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="48"/>
+    <col min="5" max="5" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="48"/>
+      <c r="H1" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="47"/>
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="47"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="47"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E8" s="49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E9" s="47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Improve filter function in view-user: Prevent send request when typing filter, only send request after 1 second. - Improve sort function in view-user - Improve account service (count-all and get-all function) for paging account in view-user - Add status column in view-user - Fix some convention in VacationController
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="100">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -231,12 +231,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>Lỗi:</t>
-  </si>
-  <si>
-    <t>server trả về lỗi khi user/pass sai, làm sao để xóa bỏ</t>
   </si>
   <si>
     <t>From 9AM to 7PM</t>
@@ -925,6 +919,9 @@
   <si>
     <t>time relax</t>
   </si>
+  <si>
+    <t>:(</t>
+  </si>
 </sst>
 </file>
 
@@ -1110,7 +1107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1266,6 +1263,8 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1282,8 +1281,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1791,7 +1790,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1823,9 +1822,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="34"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -1859,14 +1858,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -1885,7 +1884,7 @@
       </c>
       <c r="D4" s="55"/>
       <c r="E4" s="57" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F4" s="56" t="s">
         <v>64</v>
@@ -1899,14 +1898,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -1925,7 +1924,7 @@
       </c>
       <c r="D6" s="40"/>
       <c r="E6" s="52" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F6" s="52" t="s">
         <v>64</v>
@@ -1948,7 +1947,7 @@
       </c>
       <c r="D7" s="40"/>
       <c r="E7" s="52" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F7" s="43" t="s">
         <v>64</v>
@@ -1992,7 +1991,7 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="15"/>
@@ -2034,7 +2033,7 @@
       </c>
       <c r="D11" s="40"/>
       <c r="E11" s="52" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F11" s="39" t="s">
         <v>64</v>
@@ -2048,14 +2047,14 @@
       <c r="M11" s="43"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
       <c r="G12" s="15"/>
       <c r="H12" s="7"/>
       <c r="I12" s="16"/>
@@ -2107,14 +2106,14 @@
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
       <c r="G15" s="15"/>
       <c r="H15" s="7"/>
       <c r="I15" s="16"/>
@@ -2133,10 +2132,10 @@
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F16" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G16" s="51" t="s">
         <v>26</v>
@@ -2158,7 +2157,7 @@
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F17" s="32"/>
     </row>
@@ -2205,14 +2204,14 @@
       <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -15827,8 +15826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15838,161 +15837,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="59" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="65" t="s">
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="59"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="59" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="65" t="s">
+      <c r="B5" s="59" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="59" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="66" t="s">
+      <c r="B6" s="59" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="68" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="67" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="68" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="B12" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="65"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="65" t="s">
-        <v>71</v>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13" s="59" t="s">
+        <v>53</v>
       </c>
-      <c r="B5" s="65" t="s">
+    </row>
+    <row r="14" spans="1:3" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="59" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="65" t="s">
-        <v>72</v>
+      <c r="C14" s="59"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="59" t="s">
+        <v>85</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="65" t="s">
-        <v>73</v>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="59" t="s">
+        <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="65" t="s">
+      <c r="B16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="65" t="s">
-        <v>75</v>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="59" t="s">
+        <v>87</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B17" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
-        <v>76</v>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="59" t="s">
+        <v>89</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="B18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="65" t="s">
-        <v>78</v>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="59" t="s">
+        <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="65" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="65" t="s">
+      <c r="B20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C13" s="65" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="65" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="65"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="65" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="65" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="65" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="65" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="59" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="65" t="s">
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="68" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="65" t="s">
+      <c r="B22" s="59" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="68" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="65" t="s">
+      <c r="B23" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="59" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="68" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="65" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="68" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="65" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="68" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="65" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="68" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="65" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="68" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="65" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="65" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -16040,9 +16078,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -16076,14 +16114,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -16114,14 +16152,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -16152,14 +16190,14 @@
       <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
       <c r="G7" s="15"/>
       <c r="H7" s="7"/>
       <c r="I7" s="16"/>
@@ -29804,7 +29842,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
@@ -29819,13 +29857,10 @@
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C1" s="48"/>
-      <c r="H1" s="31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>42</v>
       </c>
@@ -29836,11 +29871,8 @@
         <v>57</v>
       </c>
       <c r="G2" s="47"/>
-      <c r="I2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>43</v>
       </c>
@@ -29852,7 +29884,7 @@
       </c>
       <c r="G3" s="47"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>44</v>
       </c>
@@ -29867,7 +29899,7 @@
       </c>
       <c r="G4" s="47"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>45</v>
       </c>
@@ -29878,7 +29910,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>46</v>
       </c>
@@ -29889,7 +29921,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>50</v>
       </c>
@@ -29900,17 +29932,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E8" s="49" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E9" s="47" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>47</v>
       </c>
@@ -29918,7 +29950,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>48</v>
       </c>
@@ -29929,7 +29961,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>49</v>
       </c>
@@ -29937,7 +29969,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="46" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
- Booking: Add allday option
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="98">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -267,9 +267,6 @@
   </si>
   <si>
     <t>booking by day or hour</t>
-  </si>
-  <si>
-    <t>change remaing day to hours</t>
   </si>
   <si>
     <r>
@@ -919,15 +916,12 @@
   <si>
     <t>time relax</t>
   </si>
-  <si>
-    <t>:(</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1039,12 +1033,6 @@
       <charset val="163"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="163"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF00B0F0"/>
@@ -1107,7 +1095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1263,8 +1251,8 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1283,6 +1271,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1884,7 +1876,7 @@
       </c>
       <c r="D4" s="55"/>
       <c r="E4" s="57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" s="56" t="s">
         <v>64</v>
@@ -1924,7 +1916,7 @@
       </c>
       <c r="D6" s="40"/>
       <c r="E6" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F6" s="52" t="s">
         <v>64</v>
@@ -1947,7 +1939,7 @@
       </c>
       <c r="D7" s="40"/>
       <c r="E7" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F7" s="43" t="s">
         <v>64</v>
@@ -1991,7 +1983,7 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="15"/>
@@ -2033,7 +2025,7 @@
       </c>
       <c r="D11" s="40"/>
       <c r="E11" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F11" s="39" t="s">
         <v>64</v>
@@ -2132,7 +2124,7 @@
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F16" s="32" t="s">
         <v>65</v>
@@ -2157,7 +2149,7 @@
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F17" s="32"/>
     </row>
@@ -15824,213 +15816,250 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="59"/>
+    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="71">
+        <v>42957</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="59" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="60" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="C5" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="59"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="59" t="s">
+      <c r="D5" s="60"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="C6" s="60" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="59" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="C7" s="60" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="68" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="60" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="67" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="60" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="60" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="71">
+        <v>42957</v>
+      </c>
+      <c r="D12" s="60" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="59"/>
+      <c r="B13" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="72">
+        <v>42958</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="72">
+        <v>42958</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="72">
+        <v>42958</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="72">
+        <v>42958</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="72">
+        <v>42958</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="72">
+        <v>42958</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="72">
+        <v>42958</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="72">
+        <v>42958</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="70" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="72">
+        <v>42958</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+    </row>
+    <row r="23" spans="2:4" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="68" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="67" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="59" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="67" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="59" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="68" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" s="59" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C13" s="59" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="59"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="59" t="s">
-        <v>90</v>
-      </c>
-      <c r="B20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="68" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" s="59" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="68" t="s">
+      <c r="C23"/>
+      <c r="D23" s="60"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="59" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="68" t="s">
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="68" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="68" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="68" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="68" t="s">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="68" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="68" t="s">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="68" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="68" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Add config Vacation Day (Working time and lunch break) - Improve and fix bugs: create vacation day function (using config vacation day) - Improve GetBookingVacationDay function - Add loading for create vacation day - Fix bugs: can't booking when out of vacation day
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="97">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -264,9 +264,6 @@
   </si>
   <si>
     <t>Thời hạn đổi mật khẩu đã hết (invalid token)</t>
-  </si>
-  <si>
-    <t>booking by day or hour</t>
   </si>
   <si>
     <r>
@@ -911,10 +908,10 @@
     <t>config: 12</t>
   </si>
   <si>
-    <t>time work</t>
+    <t>+time work</t>
   </si>
   <si>
-    <t>time relax</t>
+    <t>+time relax</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1092,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1253,6 +1250,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1269,12 +1273,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1782,7 +1781,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1814,9 +1813,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="34"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -1850,14 +1849,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -1876,7 +1875,7 @@
       </c>
       <c r="D4" s="55"/>
       <c r="E4" s="57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" s="56" t="s">
         <v>64</v>
@@ -1890,14 +1889,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -1916,7 +1915,7 @@
       </c>
       <c r="D6" s="40"/>
       <c r="E6" s="52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" s="52" t="s">
         <v>64</v>
@@ -1939,7 +1938,7 @@
       </c>
       <c r="D7" s="40"/>
       <c r="E7" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F7" s="43" t="s">
         <v>64</v>
@@ -1983,7 +1982,7 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="15"/>
@@ -2025,7 +2024,7 @@
       </c>
       <c r="D11" s="40"/>
       <c r="E11" s="52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F11" s="39" t="s">
         <v>64</v>
@@ -2039,14 +2038,14 @@
       <c r="M11" s="43"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
       <c r="G12" s="15"/>
       <c r="H12" s="7"/>
       <c r="I12" s="16"/>
@@ -2098,14 +2097,14 @@
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
       <c r="G15" s="15"/>
       <c r="H15" s="7"/>
       <c r="I15" s="16"/>
@@ -2124,7 +2123,7 @@
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F16" s="32" t="s">
         <v>65</v>
@@ -2149,7 +2148,7 @@
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F17" s="32"/>
     </row>
@@ -2196,14 +2195,14 @@
       <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="62"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -15818,8 +15817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15830,7 +15829,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="71">
+      <c r="A1" s="66">
         <v>42957</v>
       </c>
     </row>
@@ -15884,7 +15883,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="62" t="s">
         <v>72</v>
       </c>
       <c r="C8" s="60" t="s">
@@ -15892,7 +15891,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="62" t="s">
         <v>73</v>
       </c>
       <c r="C9" s="60" t="s">
@@ -15900,7 +15899,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="62" t="s">
         <v>74</v>
       </c>
       <c r="C10" s="60" t="s">
@@ -15916,7 +15915,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="71">
+      <c r="A12" s="66">
         <v>42957</v>
       </c>
       <c r="D12" s="60" t="s">
@@ -15926,140 +15925,166 @@
     <row r="13" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="59"/>
       <c r="B13" s="60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="72">
+      <c r="D13" s="67">
         <v>42958</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="72">
+      <c r="D14" s="67">
         <v>42958</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="72">
+      <c r="D15" s="67">
         <v>42958</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="72">
+      <c r="D16" s="67">
         <v>42958</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="72">
+      <c r="D17" s="67">
         <v>42958</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="72">
+      <c r="D18" s="67">
         <v>42958</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="72">
+      <c r="D19" s="67">
         <v>42958</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="69" t="s">
-        <v>91</v>
+      <c r="B20" s="64" t="s">
+        <v>90</v>
       </c>
       <c r="C20" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="72">
+      <c r="D20" s="67">
         <v>42958</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="70" t="s">
-        <v>92</v>
+      <c r="B21" s="65" t="s">
+        <v>91</v>
       </c>
       <c r="C21" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="72">
+      <c r="D21" s="67">
         <v>42958</v>
       </c>
     </row>
-    <row r="22" spans="2:4" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="68" t="s">
-        <v>76</v>
-      </c>
+    <row r="22" spans="2:4" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="65"/>
       <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
+      <c r="D22" s="67"/>
     </row>
     <row r="23" spans="2:4" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="C23"/>
-      <c r="D23" s="60"/>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="67">
+        <v>42961</v>
+      </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="67">
+        <v>42961</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="64" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="68" t="s">
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="67">
+        <v>42961</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="63" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="68" t="s">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="74" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="68" t="s">
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="67">
+        <v>42961</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="74" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="68" t="s">
-        <v>97</v>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="67">
+        <v>42961</v>
       </c>
     </row>
   </sheetData>
@@ -16107,9 +16132,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -16143,14 +16168,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -16181,14 +16206,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -16219,14 +16244,14 @@
       <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="15"/>
       <c r="H7" s="7"/>
       <c r="I7" s="16"/>

</xml_diff>

<commit_message>
- Add vacation duration rule - Add table VacationConfig - Fix bugs in book.controller.js
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8595" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8595"/>
   </bookViews>
   <sheets>
     <sheet name="Web" sheetId="1" r:id="rId1"/>
@@ -813,6 +813,48 @@
     </r>
   </si>
   <si>
+    <t>Route: init-new-user</t>
+  </si>
+  <si>
+    <t>Route: check-new-user</t>
+  </si>
+  <si>
+    <t>Route: get-booking</t>
+  </si>
+  <si>
+    <t>Vacation Controller</t>
+  </si>
+  <si>
+    <t>booking/userId/{userId}</t>
+  </si>
+  <si>
+    <t>Add function change password</t>
+  </si>
+  <si>
+    <t>Loading create user</t>
+  </si>
+  <si>
+    <t>page size</t>
+  </si>
+  <si>
+    <t>search: delay some seconds</t>
+  </si>
+  <si>
+    <t>hours - day</t>
+  </si>
+  <si>
+    <t>options: allday</t>
+  </si>
+  <si>
+    <t>config: 12</t>
+  </si>
+  <si>
+    <t>+time work</t>
+  </si>
+  <si>
+    <t>+time relax</t>
+  </si>
+  <si>
     <r>
       <t>'- Each employee will have 12 days off (configurable), every time a vacation booked, employee's days off will be reduce accordingly
 - Able to</t>
@@ -868,50 +910,28 @@
       <t xml:space="preserve">
 - Able to see my vacation on google calendar
 - After submited, Team Lead and HR will recieve an email notification
-- Abe to edit submited vacation, Team Lead and HR will recieve email notification</t>
+- Abe to </t>
     </r>
-  </si>
-  <si>
-    <t>Route: init-new-user</t>
-  </si>
-  <si>
-    <t>Route: check-new-user</t>
-  </si>
-  <si>
-    <t>Route: get-booking</t>
-  </si>
-  <si>
-    <t>Vacation Controller</t>
-  </si>
-  <si>
-    <t>booking/userId/{userId}</t>
-  </si>
-  <si>
-    <t>Add function change password</t>
-  </si>
-  <si>
-    <t>Loading create user</t>
-  </si>
-  <si>
-    <t>page size</t>
-  </si>
-  <si>
-    <t>search: delay some seconds</t>
-  </si>
-  <si>
-    <t>hours - day</t>
-  </si>
-  <si>
-    <t>options: allday</t>
-  </si>
-  <si>
-    <t>config: 12</t>
-  </si>
-  <si>
-    <t>+time work</t>
-  </si>
-  <si>
-    <t>+time relax</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>edit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> submited vacation, Team Lead and HR will recieve email notification</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1257,6 +1277,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1273,7 +1294,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1777,11 +1797,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M923"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="6" ySplit="2" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1813,9 +1833,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="34"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -1849,14 +1869,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -1889,14 +1909,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -2038,14 +2058,14 @@
       <c r="M11" s="43"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
       <c r="G12" s="15"/>
       <c r="H12" s="7"/>
       <c r="I12" s="16"/>
@@ -2097,14 +2117,14 @@
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
       <c r="G15" s="15"/>
       <c r="H15" s="7"/>
       <c r="I15" s="16"/>
@@ -2123,7 +2143,7 @@
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="33" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="F16" s="32" t="s">
         <v>65</v>
@@ -2195,14 +2215,14 @@
       <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="68" t="s">
+      <c r="A20" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="69"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -15817,7 +15837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -15925,7 +15945,7 @@
     <row r="13" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="59"/>
       <c r="B13" s="60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="60" t="s">
         <v>52</v>
@@ -15936,7 +15956,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
         <v>52</v>
@@ -15947,7 +15967,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
         <v>52</v>
@@ -15958,7 +15978,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
         <v>52</v>
@@ -15969,7 +15989,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" t="s">
         <v>52</v>
@@ -15980,7 +16000,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
         <v>52</v>
@@ -15991,7 +16011,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" t="s">
         <v>52</v>
@@ -16002,7 +16022,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C20" s="60" t="s">
         <v>52</v>
@@ -16013,7 +16033,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="65" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" s="60" t="s">
         <v>52</v>
@@ -16040,7 +16060,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" s="60" t="s">
         <v>52</v>
@@ -16051,7 +16071,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
@@ -16062,12 +16082,12 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="63" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="68" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="74" t="s">
-        <v>95</v>
       </c>
       <c r="C27" t="s">
         <v>52</v>
@@ -16077,8 +16097,8 @@
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="74" t="s">
-        <v>96</v>
+      <c r="B28" s="68" t="s">
+        <v>95</v>
       </c>
       <c r="C28" t="s">
         <v>52</v>
@@ -16132,9 +16152,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -16168,14 +16188,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -16206,14 +16226,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -16244,14 +16264,14 @@
       <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
       <c r="G7" s="15"/>
       <c r="H7" s="7"/>
       <c r="I7" s="16"/>

</xml_diff>

<commit_message>
- Add vacation config
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="98">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -146,11 +146,6 @@
   </si>
   <si>
     <t>As a admin, I want to set the rule of vacation booking</t>
-  </si>
-  <si>
-    <t>- If vacation duration &gt; 1 and &lt; 5 days, do not allow to book winthin a week
-- If vacation duration &gt; 5 do not allow book within a month
-- Number of duration in the rules need to be configurable (e.g: 4 days, 5 days)</t>
   </si>
   <si>
     <t>Report</t>
@@ -932,6 +927,116 @@
       </rPr>
       <t xml:space="preserve"> submited vacation, Team Lead and HR will recieve email notification</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- If vacation duration </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>&gt; 1 and &lt; 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> days, do not allow to book </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>winthin a week</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">
+- If vacation duration </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>&gt; 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> do not allow book </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>within a month</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">
+- Number of duration in the rules need to be </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>configurable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g: 4 days, 5 days)</t>
+    </r>
+  </si>
+  <si>
+    <t>Not yet</t>
   </si>
 </sst>
 </file>
@@ -1801,7 +1906,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1895,10 +2000,10 @@
       </c>
       <c r="D4" s="55"/>
       <c r="E4" s="57" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="7"/>
@@ -1935,10 +2040,10 @@
       </c>
       <c r="D6" s="40"/>
       <c r="E6" s="52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="7"/>
@@ -1958,10 +2063,10 @@
       </c>
       <c r="D7" s="40"/>
       <c r="E7" s="52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="7"/>
@@ -2002,7 +2107,7 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="15"/>
@@ -2044,10 +2149,10 @@
       </c>
       <c r="D11" s="40"/>
       <c r="E11" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G11" s="41"/>
       <c r="H11" s="42"/>
@@ -2105,7 +2210,7 @@
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="15"/>
@@ -2143,10 +2248,10 @@
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G16" s="51" t="s">
         <v>26</v>
@@ -2168,7 +2273,7 @@
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F17" s="32"/>
     </row>
@@ -2194,18 +2299,20 @@
       <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="23"/>
-      <c r="B19" s="19" t="s">
+      <c r="A19" s="37"/>
+      <c r="B19" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="33" t="s">
-        <v>38</v>
+      <c r="D19" s="40"/>
+      <c r="E19" s="52" t="s">
+        <v>96</v>
       </c>
-      <c r="F19" s="32"/>
+      <c r="F19" s="39" t="s">
+        <v>97</v>
+      </c>
       <c r="G19" s="15"/>
       <c r="H19" s="7"/>
       <c r="I19" s="16"/>
@@ -2216,7 +2323,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="69" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="70"/>
       <c r="C20" s="70"/>
@@ -2237,11 +2344,11 @@
         <v>9</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="15" t="s">
@@ -15855,83 +15962,83 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="C2" t="s">
-        <v>52</v>
+      <c r="C3" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="60" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="C3" t="s">
-        <v>52</v>
+      <c r="C4" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="60" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="60"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="C4" t="s">
-        <v>52</v>
+      <c r="C6" s="60" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="60" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="60"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="60" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="60" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="60" t="s">
-        <v>70</v>
-      </c>
       <c r="C7" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="60" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="60" t="s">
-        <v>52</v>
+      <c r="C9" s="60" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="62" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="60" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="62" t="s">
-        <v>74</v>
-      </c>
       <c r="C10" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -15939,16 +16046,16 @@
         <v>42957</v>
       </c>
       <c r="D12" s="60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="59"/>
       <c r="B13" s="60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="67">
         <v>42958</v>
@@ -15956,10 +16063,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" s="67">
         <v>42958</v>
@@ -15967,10 +16074,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" s="67">
         <v>42958</v>
@@ -15978,10 +16085,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" s="67">
         <v>42958</v>
@@ -15989,10 +16096,10 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="67">
         <v>42958</v>
@@ -16000,10 +16107,10 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" s="67">
         <v>42958</v>
@@ -16011,10 +16118,10 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="67">
         <v>42958</v>
@@ -16022,10 +16129,10 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="64" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20" s="67">
         <v>42958</v>
@@ -16033,10 +16140,10 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="67">
         <v>42958</v>
@@ -16049,10 +16156,10 @@
     </row>
     <row r="23" spans="2:4" s="59" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="67">
         <v>42961</v>
@@ -16060,10 +16167,10 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="64" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="67">
         <v>42961</v>
@@ -16071,10 +16178,10 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" s="67">
         <v>42961</v>
@@ -16082,15 +16189,15 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="63" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="68" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="68" t="s">
-        <v>94</v>
-      </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D27" s="67">
         <v>42961</v>
@@ -16098,10 +16205,10 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="68" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28" s="67">
         <v>42961</v>
@@ -29936,116 +30043,116 @@
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="47"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="48" t="s">
-        <v>52</v>
+      <c r="C3" s="48" t="s">
+        <v>51</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="E3" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="47"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="47"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="47"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>43</v>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>49</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>52</v>
+      <c r="C7" s="48" t="s">
+        <v>51</v>
       </c>
-      <c r="E3" s="49" t="s">
-        <v>54</v>
+      <c r="E7" s="49" t="s">
+        <v>58</v>
       </c>
-      <c r="G3" s="47"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>44</v>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E8" s="49" t="s">
+        <v>59</v>
       </c>
-      <c r="C4" s="48" t="s">
-        <v>52</v>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E9" s="47" t="s">
+        <v>60</v>
       </c>
-      <c r="E4" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="47"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="47" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="49" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="49" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E8" s="49" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E9" s="47" t="s">
+      <c r="E10" s="49" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="C11" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="49" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
       <c r="C12" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Fix bugs: Vacation duration
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="97">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -1035,9 +1035,6 @@
       <t xml:space="preserve"> (e.g: 4 days, 5 days)</t>
     </r>
   </si>
-  <si>
-    <t>Not yet</t>
-  </si>
 </sst>
 </file>
 
@@ -1217,7 +1214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1335,19 +1332,9 @@
     <xf numFmtId="4" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1399,6 +1386,19 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1906,7 +1906,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1938,9 +1938,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="34"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -1974,14 +1974,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -1991,18 +1991,18 @@
       <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="53"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="57" t="s">
+      <c r="D4" s="51"/>
+      <c r="E4" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="52" t="s">
         <v>63</v>
       </c>
       <c r="G4" s="15"/>
@@ -2014,14 +2014,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -2039,10 +2039,10 @@
         <v>14</v>
       </c>
       <c r="D6" s="40"/>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="52" t="s">
+      <c r="F6" s="48" t="s">
         <v>63</v>
       </c>
       <c r="G6" s="15"/>
@@ -2062,10 +2062,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="40"/>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="41" t="s">
         <v>63</v>
       </c>
       <c r="G7" s="15"/>
@@ -2139,7 +2139,7 @@
       <c r="L10" s="16"/>
       <c r="M10" s="16"/>
     </row>
-    <row r="11" spans="1:13" s="45" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="75" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="37"/>
       <c r="B11" s="38" t="s">
         <v>9</v>
@@ -2148,29 +2148,29 @@
         <v>29</v>
       </c>
       <c r="D11" s="40"/>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="48" t="s">
         <v>79</v>
       </c>
       <c r="F11" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="41"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
       <c r="G12" s="15"/>
       <c r="H12" s="7"/>
       <c r="I12" s="16"/>
@@ -2222,14 +2222,14 @@
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="69" t="s">
+      <c r="A15" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
       <c r="G15" s="15"/>
       <c r="H15" s="7"/>
       <c r="I15" s="16"/>
@@ -2243,7 +2243,7 @@
       <c r="B16" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="46" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="24"/>
@@ -2253,7 +2253,7 @@
       <c r="F16" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="51" t="s">
+      <c r="G16" s="47" t="s">
         <v>26</v>
       </c>
       <c r="H16" s="7"/>
@@ -2307,11 +2307,11 @@
         <v>37</v>
       </c>
       <c r="D19" s="40"/>
-      <c r="E19" s="52" t="s">
+      <c r="E19" s="48" t="s">
         <v>96</v>
       </c>
       <c r="F19" s="39" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="7"/>
@@ -2322,14 +2322,14 @@
       <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -15950,18 +15950,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="59"/>
+    <col min="1" max="1" width="9.140625" style="55"/>
     <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="66">
+    <row r="1" spans="1:4" s="55" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="62">
         <v>42957</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="56" t="s">
         <v>65</v>
       </c>
       <c r="C2" t="s">
@@ -15969,7 +15969,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="56" t="s">
         <v>66</v>
       </c>
       <c r="C3" t="s">
@@ -15977,7 +15977,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="56" t="s">
         <v>67</v>
       </c>
       <c r="C4" t="s">
@@ -15985,232 +15985,232 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="60"/>
+      <c r="D5" s="56"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="56" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="56" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="56" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="56" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="56" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="56" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="66">
+      <c r="A12" s="62">
         <v>42957</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="56" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="59"/>
-      <c r="B13" s="60" t="s">
+    <row r="13" spans="1:4" s="54" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="55"/>
+      <c r="B13" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="67">
+      <c r="D13" s="63">
         <v>42958</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="56" t="s">
         <v>81</v>
       </c>
       <c r="C14" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="67">
+      <c r="D14" s="63">
         <v>42958</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="56" t="s">
         <v>82</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="67">
+      <c r="D15" s="63">
         <v>42958</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="56" t="s">
         <v>83</v>
       </c>
       <c r="C16" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="67">
+      <c r="D16" s="63">
         <v>42958</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="56" t="s">
         <v>85</v>
       </c>
       <c r="C17" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="67">
+      <c r="D17" s="63">
         <v>42958</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="56" t="s">
         <v>86</v>
       </c>
       <c r="C18" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="67">
+      <c r="D18" s="63">
         <v>42958</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="56" t="s">
         <v>87</v>
       </c>
       <c r="C19" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="67">
+      <c r="D19" s="63">
         <v>42958</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="67">
+      <c r="D20" s="63">
         <v>42958</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="67">
+      <c r="D21" s="63">
         <v>42958</v>
       </c>
     </row>
-    <row r="22" spans="2:4" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="65"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="67"/>
-    </row>
-    <row r="23" spans="2:4" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="64" t="s">
+    <row r="22" spans="2:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="61"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="63"/>
+    </row>
+    <row r="23" spans="2:4" s="55" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="60" t="s">
         <v>70</v>
       </c>
       <c r="C23" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="67">
+      <c r="D23" s="63">
         <v>42961</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="64" t="s">
+      <c r="B24" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="C24" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="67">
+      <c r="D24" s="63">
         <v>42961</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="60" t="s">
         <v>91</v>
       </c>
       <c r="C25" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="67">
+      <c r="D25" s="63">
         <v>42961</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="63" t="s">
+      <c r="B26" s="59" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="64" t="s">
         <v>93</v>
       </c>
       <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="67">
+      <c r="D27" s="63">
         <v>42961</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="68" t="s">
+      <c r="B28" s="64" t="s">
         <v>94</v>
       </c>
       <c r="C28" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="67">
+      <c r="D28" s="63">
         <v>42961</v>
       </c>
     </row>
@@ -16259,9 +16259,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -16295,14 +16295,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -16333,14 +16333,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -16371,14 +16371,14 @@
       <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
       <c r="G7" s="15"/>
       <c r="H7" s="7"/>
       <c r="I7" s="16"/>
@@ -30033,61 +30033,61 @@
   <cols>
     <col min="1" max="1" width="9.140625" style="31"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="48"/>
+    <col min="3" max="3" width="9.140625" style="44"/>
     <col min="5" max="5" width="56.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="48"/>
+      <c r="C1" s="44"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="E2" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="47"/>
+      <c r="G2" s="43"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="47"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="47" t="s">
+      <c r="F4" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="47"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="43" t="s">
         <v>55</v>
       </c>
     </row>
@@ -30095,10 +30095,10 @@
       <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="45" t="s">
         <v>57</v>
       </c>
     </row>
@@ -30106,20 +30106,20 @@
       <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="49" t="s">
+      <c r="E7" s="45" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="45" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E9" s="47" t="s">
+      <c r="E9" s="43" t="s">
         <v>60</v>
       </c>
     </row>
@@ -30127,7 +30127,7 @@
       <c r="B10" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="45" t="s">
         <v>61</v>
       </c>
     </row>
@@ -30135,10 +30135,10 @@
       <c r="B11" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="45" t="s">
         <v>62</v>
       </c>
     </row>
@@ -30146,12 +30146,12 @@
       <c r="B12" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="44" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="42" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Update user information
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -748,31 +748,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">'- Able to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>reset password</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> by input the email</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>- Able to</t>
     </r>
     <r>
@@ -848,85 +823,6 @@
   </si>
   <si>
     <t>+time relax</t>
-  </si>
-  <si>
-    <r>
-      <t>'- Each employee will have 12 days off (configurable), every time a vacation booked, employee's days off will be reduce accordingly
-- Able to</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>book vacation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> with some information such as: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>from date - to date, from hour - to hour, reason</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">
-- Able to see my vacation on google calendar
-- After submited, Team Lead and HR will recieve an email notification
-- Abe to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>edit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> submited vacation, Team Lead and HR will recieve email notification</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1033,6 +929,110 @@
         <charset val="163"/>
       </rPr>
       <t xml:space="preserve"> (e.g: 4 days, 5 days)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>- Each employee will have 12 days off (configurable), every time a vacation booked, employee's days off will be reduce accordingly
+- Able to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>book vacation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> with some information such as: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>from date - to date, from hour - to hour, reason</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">
+- Able to see my vacation on google calendar
+- After submited, Team Lead and HR will recieve an email notification
+- Abe to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>edit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> submited vacation, Team Lead and HR will recieve email notification</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>reset password</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> by input the email</t>
     </r>
   </si>
 </sst>
@@ -1903,10 +1903,10 @@
   <dimension ref="A1:M923"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20:F20"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1916,7 +1916,7 @@
     <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="112.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="31" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="31" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="25.85546875" customWidth="1"/>
     <col min="10" max="10" width="19.140625" customWidth="1"/>
     <col min="11" max="11" width="21.28515625" customWidth="1"/>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="D11" s="40"/>
       <c r="E11" s="48" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="F11" s="39" t="s">
         <v>63</v>
@@ -2273,7 +2273,7 @@
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F17" s="32"/>
     </row>
@@ -2308,7 +2308,7 @@
       </c>
       <c r="D19" s="40"/>
       <c r="E19" s="48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F19" s="39" t="s">
         <v>63</v>
@@ -16052,7 +16052,7 @@
     <row r="13" spans="1:4" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="55"/>
       <c r="B13" s="56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" s="56" t="s">
         <v>51</v>
@@ -16063,7 +16063,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
         <v>51</v>
@@ -16074,7 +16074,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
@@ -16085,7 +16085,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s">
         <v>51</v>
@@ -16096,7 +16096,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="56" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17" t="s">
         <v>51</v>
@@ -16107,7 +16107,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
         <v>51</v>
@@ -16118,7 +16118,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
         <v>51</v>
@@ -16129,7 +16129,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" s="56" t="s">
         <v>51</v>
@@ -16140,7 +16140,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="56" t="s">
         <v>51</v>
@@ -16167,7 +16167,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" s="56" t="s">
         <v>51</v>
@@ -16178,7 +16178,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="60" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
         <v>51</v>
@@ -16189,12 +16189,12 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="59" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
         <v>51</v>
@@ -16205,7 +16205,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="64" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
- Send email after booking - Fix some bugs
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="97">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -680,74 +680,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">- Able to edit all general information: Name, DoB, Gender, Picture, Remaining days off...
-- Able to set employee to a deparment
-- Able to set employee to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>inactive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> if he/she is active state and then employee </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>can't login</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> into system
-- Able to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>reactivate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> employee account</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>- Able to</t>
     </r>
     <r>
@@ -933,6 +865,179 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>reset password</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> by input the email</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>edit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> all general information: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>Name, DoB, Gender, Picture, Remaining days off...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">
+- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>set</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> employee to a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>deparment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">
+- Able to set employee to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>inactive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> if he/she is active state and then employee </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>can't login</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> into system
+- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>reactivate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> employee account</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>- Each employee will have 12 days off (configurable), every time a vacation booked, employee's days off will be reduce accordingly
 - Able to</t>
     </r>
@@ -986,7 +1091,47 @@
       </rPr>
       <t xml:space="preserve">
 - Able to see my vacation on google calendar
-- After submited, Team Lead and HR will recieve an email notification
+- After </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>submited,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> Team Lead and HR will recieve an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> notification
 - Abe to </t>
     </r>
     <r>
@@ -1008,31 +1153,6 @@
         <charset val="163"/>
       </rPr>
       <t xml:space="preserve"> submited vacation, Team Lead and HR will recieve email notification</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">- Able to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>reset password</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> by input the email</t>
     </r>
   </si>
 </sst>
@@ -1214,7 +1334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1370,6 +1490,19 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1386,19 +1519,21 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1903,19 +2038,19 @@
   <dimension ref="A1:M923"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="112.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="108.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="31" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="25.85546875" customWidth="1"/>
     <col min="10" max="10" width="19.140625" customWidth="1"/>
@@ -1938,9 +2073,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="34"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -1974,14 +2109,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -2014,14 +2149,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -2097,49 +2232,51 @@
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
     </row>
-    <row r="9" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
-      <c r="B9" s="19" t="s">
+    <row r="9" spans="1:13" s="69" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="37"/>
+      <c r="B9" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="33" t="s">
-        <v>78</v>
+      <c r="D9" s="40"/>
+      <c r="E9" s="48" t="s">
+        <v>95</v>
       </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="19" t="s">
+      <c r="F9" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="65"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
+      <c r="M9" s="67"/>
+    </row>
+    <row r="10" spans="1:13" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="76"/>
+      <c r="B10" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="33" t="s">
+      <c r="D10" s="78"/>
+      <c r="E10" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-    </row>
-    <row r="11" spans="1:13" s="75" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F10" s="80"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="67"/>
+      <c r="M10" s="67"/>
+    </row>
+    <row r="11" spans="1:13" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="37"/>
       <c r="B11" s="38" t="s">
         <v>9</v>
@@ -2149,28 +2286,28 @@
       </c>
       <c r="D11" s="40"/>
       <c r="E11" s="48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F11" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="71"/>
-      <c r="H11" s="72"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="70" t="s">
+      <c r="A12" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
       <c r="G12" s="15"/>
       <c r="H12" s="7"/>
       <c r="I12" s="16"/>
@@ -2222,14 +2359,14 @@
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
       <c r="G15" s="15"/>
       <c r="H15" s="7"/>
       <c r="I15" s="16"/>
@@ -2238,7 +2375,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A16" s="23"/>
       <c r="B16" s="19" t="s">
         <v>9</v>
@@ -2248,7 +2385,7 @@
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="33" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F16" s="32" t="s">
         <v>64</v>
@@ -2273,7 +2410,7 @@
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F17" s="32"/>
     </row>
@@ -2308,7 +2445,7 @@
       </c>
       <c r="D19" s="40"/>
       <c r="E19" s="48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F19" s="39" t="s">
         <v>63</v>
@@ -2322,14 +2459,14 @@
       <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -16052,7 +16189,7 @@
     <row r="13" spans="1:4" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="55"/>
       <c r="B13" s="56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13" s="56" t="s">
         <v>51</v>
@@ -16063,7 +16200,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
         <v>51</v>
@@ -16074,7 +16211,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
@@ -16085,7 +16222,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
         <v>51</v>
@@ -16096,7 +16233,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
         <v>51</v>
@@ -16107,7 +16244,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="56" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" t="s">
         <v>51</v>
@@ -16118,7 +16255,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
         <v>51</v>
@@ -16129,7 +16266,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="56" t="s">
         <v>51</v>
@@ -16140,7 +16277,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="56" t="s">
         <v>51</v>
@@ -16167,7 +16304,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C24" s="56" t="s">
         <v>51</v>
@@ -16178,7 +16315,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
         <v>51</v>
@@ -16189,12 +16326,12 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="59" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
         <v>51</v>
@@ -16205,7 +16342,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
         <v>51</v>
@@ -16259,9 +16396,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -16295,14 +16432,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -16333,14 +16470,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -16371,14 +16508,14 @@
       <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
       <c r="G7" s="15"/>
       <c r="H7" s="7"/>
       <c r="I7" s="16"/>

</xml_diff>

<commit_message>
- Update edit booking - Update report
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="105">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -1049,10 +1049,158 @@
     </r>
   </si>
   <si>
-    <t>Turned off send email</t>
+    <t>Done, turned off send email</t>
   </si>
   <si>
-    <t>Done, turned off send email</t>
+    <r>
+      <t xml:space="preserve">- Able to see </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>list of day off</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>calendar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> that </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>grouped by month</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">
+- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>filter by employee</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve">
+- Able to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>see</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>remaning day</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t xml:space="preserve"> of employee</t>
+    </r>
+  </si>
+  <si>
+    <t>ừ mày có thể dùng chung bảng booking hiện tại cho admin thêm booking</t>
+  </si>
+  <si>
+    <t>nhưng mà nó có thêm 1 cột là type= admin book or user book</t>
+  </si>
+  <si>
+    <t>nếu admin book thì ghi trực tiếp số giờ vào</t>
+  </si>
+  <si>
+    <t>user book thì chọn ngày</t>
+  </si>
+  <si>
+    <t>Do tao tách admin và user, nên phần edit user chỉ có admin có, thằng user bị mất, nên tao phải làm thêm page edit cho user nữa.</t>
+  </si>
+  <si>
+    <t>năm 2017? 2018</t>
+  </si>
+  <si>
+    <t>Ờ mài, còn cái edit booking tao chưa có làm.</t>
+  </si>
+  <si>
+    <t>calendar</t>
   </si>
   <si>
     <r>
@@ -1230,43 +1378,7 @@
         <charset val="163"/>
       </rPr>
       <t xml:space="preserve"> notification
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">- Abe to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>edit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> submited vacation, Team Lead and HR will recieve email notification</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">- Able to see </t>
+- Abe to </t>
     </r>
     <r>
       <rPr>
@@ -1277,7 +1389,7 @@
         <family val="2"/>
         <charset val="163"/>
       </rPr>
-      <t>list of day off</t>
+      <t>edit</t>
     </r>
     <r>
       <rPr>
@@ -1286,27 +1398,7 @@
         <family val="2"/>
         <charset val="163"/>
       </rPr>
-      <t xml:space="preserve"> on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>calendar</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> that </t>
+      <t xml:space="preserve"> submited vacation, Team Lead and HR will </t>
     </r>
     <r>
       <rPr>
@@ -1317,7 +1409,7 @@
         <family val="2"/>
         <charset val="163"/>
       </rPr>
-      <t>grouped by month</t>
+      <t xml:space="preserve">recieve email </t>
     </r>
     <r>
       <rPr>
@@ -1326,69 +1418,7 @@
         <family val="2"/>
         <charset val="163"/>
       </rPr>
-      <t xml:space="preserve">
-- Able to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>filter by employee</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">
-- Able to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>see</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t>remaning day</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> of employee</t>
+      <t>notification</t>
     </r>
   </si>
 </sst>
@@ -1523,7 +1553,7 @@
       <charset val="163"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1545,12 +1575,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1576,7 +1600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1763,34 +1787,13 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2295,10 +2298,10 @@
   <dimension ref="A1:M923"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2632,30 +2635,30 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13" s="85" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="76"/>
-      <c r="B16" s="77" t="s">
+    <row r="16" spans="1:13" s="63" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="34"/>
+      <c r="B16" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="78" t="s">
+      <c r="C16" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="79"/>
-      <c r="E16" s="80" t="s">
-        <v>96</v>
+      <c r="D16" s="37"/>
+      <c r="E16" s="43" t="s">
+        <v>104</v>
       </c>
-      <c r="F16" s="81" t="s">
+      <c r="F16" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="82" t="s">
+      <c r="G16" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="83"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="81"/>
-      <c r="L16" s="81"/>
-      <c r="M16" s="81"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
     </row>
     <row r="17" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="34"/>
@@ -2670,7 +2673,7 @@
         <v>93</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
@@ -2744,7 +2747,7 @@
       </c>
       <c r="D21" s="37"/>
       <c r="E21" s="43" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F21" s="38" t="s">
         <v>62</v>
@@ -16340,10 +16343,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16492,7 +16495,7 @@
         <v>42958</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="50" t="s">
         <v>80</v>
       </c>
@@ -16503,7 +16506,7 @@
         <v>42958</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="50" t="s">
         <v>81</v>
       </c>
@@ -16514,7 +16517,7 @@
         <v>42958</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="50" t="s">
         <v>82</v>
       </c>
@@ -16525,7 +16528,7 @@
         <v>42958</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="54" t="s">
         <v>83</v>
       </c>
@@ -16536,7 +16539,7 @@
         <v>42958</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="55" t="s">
         <v>84</v>
       </c>
@@ -16547,12 +16550,12 @@
         <v>42958</v>
       </c>
     </row>
-    <row r="22" spans="2:4" s="51" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="55"/>
       <c r="C22" s="50"/>
       <c r="D22" s="57"/>
     </row>
-    <row r="23" spans="2:4" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="54" t="s">
         <v>68</v>
       </c>
@@ -16563,7 +16566,7 @@
         <v>42961</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="54" t="s">
         <v>85</v>
       </c>
@@ -16574,7 +16577,7 @@
         <v>42961</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="54" t="s">
         <v>86</v>
       </c>
@@ -16585,12 +16588,12 @@
         <v>42961</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="53" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="58" t="s">
         <v>88</v>
       </c>
@@ -16601,7 +16604,7 @@
         <v>42961</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="58" t="s">
         <v>89</v>
       </c>
@@ -16610,6 +16613,61 @@
       </c>
       <c r="D28" s="57">
         <v>42961</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="49">
+        <v>1</v>
+      </c>
+      <c r="B30" s="50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="49">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="49">
+        <v>3</v>
+      </c>
+      <c r="B37" s="50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="49">
+        <v>4</v>
+      </c>
+      <c r="B39" s="78" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="49">
+        <v>5</v>
+      </c>
+      <c r="B41" s="50" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Add default user in init projecct - Add edit user
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vacation\VacationTracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Company\Futurify\Project\Vacation\VacationTracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,13 +17,13 @@
     <sheet name="Mobile" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="107">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -1421,12 +1421,18 @@
       <t>notification</t>
     </r>
   </si>
+  <si>
+    <t>Remaining Days Off, for new user maybe error</t>
+  </si>
+  <si>
+    <t>with set default 12 days off for new user, must be F5 page???</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1552,6 +1558,12 @@
       <family val="2"/>
       <charset val="163"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1600,7 +1612,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1753,24 +1765,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1787,13 +1794,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2298,10 +2301,10 @@
   <dimension ref="A1:M923"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2311,7 +2314,7 @@
     <col min="3" max="3" width="47.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="108.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="65" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="25.85546875" customWidth="1"/>
     <col min="10" max="10" width="19.140625" customWidth="1"/>
     <col min="11" max="11" width="21.28515625" customWidth="1"/>
@@ -2333,9 +2336,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="30"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -2369,14 +2372,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -2397,7 +2400,7 @@
       <c r="E4" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="68" t="s">
+      <c r="F4" s="64" t="s">
         <v>62</v>
       </c>
       <c r="G4" s="15"/>
@@ -2409,14 +2412,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -2516,18 +2519,20 @@
       <c r="M9" s="61"/>
     </row>
     <row r="10" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="64"/>
-      <c r="B10" s="65" t="s">
+      <c r="A10" s="34"/>
+      <c r="B10" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="66"/>
-      <c r="E10" s="67" t="s">
+      <c r="D10" s="37"/>
+      <c r="E10" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="61"/>
+      <c r="F10" s="38" t="s">
+        <v>62</v>
+      </c>
       <c r="G10" s="59"/>
       <c r="H10" s="60"/>
       <c r="I10" s="61"/>
@@ -2560,14 +2565,14 @@
       <c r="M11" s="61"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
       <c r="G12" s="15"/>
       <c r="H12" s="7"/>
       <c r="I12" s="16"/>
@@ -2619,14 +2624,14 @@
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
       <c r="G15" s="15"/>
       <c r="H15" s="7"/>
       <c r="I15" s="16"/>
@@ -2640,7 +2645,7 @@
       <c r="B16" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="76" t="s">
+      <c r="C16" s="66" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="37"/>
@@ -2650,7 +2655,7 @@
       <c r="F16" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="77" t="s">
+      <c r="G16" s="67" t="s">
         <v>26</v>
       </c>
       <c r="H16" s="60"/>
@@ -2721,14 +2726,14 @@
       <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -16343,9 +16348,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -16495,7 +16500,7 @@
         <v>42958</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="50" t="s">
         <v>80</v>
       </c>
@@ -16506,7 +16511,7 @@
         <v>42958</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="50" t="s">
         <v>81</v>
       </c>
@@ -16517,7 +16522,7 @@
         <v>42958</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="50" t="s">
         <v>82</v>
       </c>
@@ -16528,7 +16533,7 @@
         <v>42958</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="54" t="s">
         <v>83</v>
       </c>
@@ -16539,7 +16544,7 @@
         <v>42958</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="55" t="s">
         <v>84</v>
       </c>
@@ -16550,12 +16555,12 @@
         <v>42958</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" s="51" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="55"/>
       <c r="C22" s="50"/>
       <c r="D22" s="57"/>
     </row>
-    <row r="23" spans="1:4" s="49" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="54" t="s">
         <v>68</v>
       </c>
@@ -16566,7 +16571,7 @@
         <v>42961</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="54" t="s">
         <v>85</v>
       </c>
@@ -16577,7 +16582,7 @@
         <v>42961</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="54" t="s">
         <v>86</v>
       </c>
@@ -16588,12 +16593,12 @@
         <v>42961</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="53" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="58" t="s">
         <v>88</v>
       </c>
@@ -16604,7 +16609,7 @@
         <v>42961</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="58" t="s">
         <v>89</v>
       </c>
@@ -16615,20 +16620,17 @@
         <v>42961</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="49">
-        <v>1</v>
-      </c>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="50" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>98</v>
       </c>
@@ -16639,39 +16641,46 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="49">
-        <v>2</v>
+      <c r="A35" s="76" t="s">
+        <v>50</v>
       </c>
       <c r="B35" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="49">
-        <v>3</v>
-      </c>
       <c r="B37" s="50" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="49">
-        <v>4</v>
+      <c r="A39" s="76" t="s">
+        <v>50</v>
       </c>
-      <c r="B39" s="78" t="s">
+      <c r="B39" s="68" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="49">
-        <v>5</v>
-      </c>
       <c r="B41" s="50" t="s">
         <v>103</v>
       </c>
     </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="76"/>
+      <c r="B43" s="75" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="76"/>
+      <c r="B44" s="77" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16715,9 +16724,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -16751,14 +16760,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -16789,14 +16798,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -16827,14 +16836,14 @@
       <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
       <c r="G7" s="15"/>
       <c r="H7" s="7"/>
       <c r="I7" s="16"/>

</xml_diff>

<commit_message>
- Edit role for accout controller - Fix bugs: reset-password - Fix bugs: init config vacation duration
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8595" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Web" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="Mobile" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
+    <sheet name="Function" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="155">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -1427,12 +1428,156 @@
   <si>
     <t>with set default 12 days off for new user, must be F5 page???</t>
   </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>Incorrect email or password</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Forgot password</t>
+  </si>
+  <si>
+    <t>The account cannot be found</t>
+  </si>
+  <si>
+    <t>Please check your email</t>
+  </si>
+  <si>
+    <t>Redirect Page</t>
+  </si>
+  <si>
+    <t>Booking</t>
+  </si>
+  <si>
+    <t>Reset password</t>
+  </si>
+  <si>
+    <t>Password reset successfully! Redirectly to login page…</t>
+  </si>
+  <si>
+    <t>The token is expired</t>
+  </si>
+  <si>
+    <t>Forget password</t>
+  </si>
+  <si>
+    <t>Change password</t>
+  </si>
+  <si>
+    <t>Old password is incorrect</t>
+  </si>
+  <si>
+    <t>Password was changed! Loging out…</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Config</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Update (Admin)</t>
+  </si>
+  <si>
+    <t>Update (User)</t>
+  </si>
+  <si>
+    <t>The email has been used by another user</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Send mail</t>
+  </si>
+  <si>
+    <t>Add user success!</t>
+  </si>
+  <si>
+    <t>Expect</t>
+  </si>
+  <si>
+    <t>Add to top table</t>
+  </si>
+  <si>
+    <t>Remove at table</t>
+  </si>
+  <si>
+    <t>Update user success!</t>
+  </si>
+  <si>
+    <t>Update at table</t>
+  </si>
+  <si>
+    <t>Filter user</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>Sort user</t>
+  </si>
+  <si>
+    <t>Set department</t>
+  </si>
+  <si>
+    <t>Update at table, user can't login</t>
+  </si>
+  <si>
+    <t>Set system admin</t>
+  </si>
+  <si>
+    <t>Have/haven't admin rights.</t>
+  </si>
+  <si>
+    <t>Filter by keyword</t>
+  </si>
+  <si>
+    <t>Set active/re-active</t>
+  </si>
+  <si>
+    <t>Vacation duration</t>
+  </si>
+  <si>
+    <t>In week, in month, configurable</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1564,8 +1709,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1590,8 +1742,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1608,11 +1766,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1778,6 +1988,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1794,9 +2008,38 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2300,11 +2543,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M923"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="6" ySplit="2" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2314,8 +2557,9 @@
     <col min="3" max="3" width="47.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="108.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="65" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="25.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="65" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="25.85546875" customWidth="1"/>
     <col min="10" max="10" width="19.140625" customWidth="1"/>
     <col min="11" max="11" width="21.28515625" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" customWidth="1"/>
@@ -2336,9 +2580,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="30"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -2363,7 +2607,9 @@
       <c r="F2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="11"/>
+      <c r="G2" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="14"/>
@@ -2372,14 +2618,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -2412,14 +2658,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -2565,14 +2811,14 @@
       <c r="M11" s="61"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
       <c r="G12" s="15"/>
       <c r="H12" s="7"/>
       <c r="I12" s="16"/>
@@ -2624,14 +2870,14 @@
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="69" t="s">
+      <c r="A15" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
       <c r="G15" s="15"/>
       <c r="H15" s="7"/>
       <c r="I15" s="16"/>
@@ -2726,14 +2972,14 @@
       <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -16641,7 +16887,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="76" t="s">
+      <c r="A35" s="71" t="s">
         <v>50</v>
       </c>
       <c r="B35" t="s">
@@ -16654,7 +16900,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="76" t="s">
+      <c r="A39" s="71" t="s">
         <v>50</v>
       </c>
       <c r="B39" s="68" t="s">
@@ -16667,14 +16913,14 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="76"/>
-      <c r="B43" s="75" t="s">
+      <c r="A43" s="71"/>
+      <c r="B43" s="70" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="76"/>
-      <c r="B44" s="77" t="s">
+      <c r="A44" s="71"/>
+      <c r="B44" s="72" t="s">
         <v>106</v>
       </c>
     </row>
@@ -16724,9 +16970,9 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
       <c r="J1" s="8"/>
       <c r="K1" s="9"/>
       <c r="L1" s="10"/>
@@ -16760,14 +17006,14 @@
       <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
       <c r="G3" s="15"/>
       <c r="H3" s="7"/>
       <c r="I3" s="16"/>
@@ -16798,14 +17044,14 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
       <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="16"/>
@@ -16836,14 +17082,14 @@
       <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
       <c r="G7" s="15"/>
       <c r="H7" s="7"/>
       <c r="I7" s="16"/>
@@ -30624,4 +30870,375 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="69"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="84" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="84" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="84" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="84" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="84" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="84" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" s="84" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="79" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="80"/>
+      <c r="F3" s="79" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="82"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="79" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="82"/>
+      <c r="C5" s="80" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="79" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="80"/>
+      <c r="F5" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="82"/>
+      <c r="C6" s="79" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="79" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="79" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="80"/>
+      <c r="G6" s="79" t="s">
+        <v>137</v>
+      </c>
+      <c r="H6" s="80"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="82"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="79" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="82"/>
+      <c r="C8" s="79" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="79" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="79" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="82"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="79" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="79" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="82"/>
+      <c r="C10" s="79" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="79" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="79" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="83"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="79" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="90" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="79" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="86" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="86" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" s="80"/>
+      <c r="G12" s="79" t="s">
+        <v>137</v>
+      </c>
+      <c r="H12" s="79" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="91"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="86" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="87" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="80"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="91"/>
+      <c r="C14" s="86" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="86" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="79" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="91"/>
+      <c r="C15" s="86" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="86" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="79" t="s">
+        <v>142</v>
+      </c>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="79" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="91"/>
+      <c r="C16" s="86" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="86" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="79" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+    </row>
+    <row r="17" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="91"/>
+      <c r="C17" s="86" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="86"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="86" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="91"/>
+      <c r="C18" s="86" t="s">
+        <v>147</v>
+      </c>
+      <c r="D18" s="86"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="80"/>
+      <c r="H18" s="89"/>
+    </row>
+    <row r="19" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="91"/>
+      <c r="C19" s="86" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" s="86"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="89" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="91"/>
+      <c r="C20" s="86" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" s="86"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="80"/>
+    </row>
+    <row r="21" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="91"/>
+      <c r="C21" s="86" t="s">
+        <v>144</v>
+      </c>
+      <c r="D21" s="86"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="80"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="79" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="92"/>
+      <c r="C22" s="86" t="s">
+        <v>146</v>
+      </c>
+      <c r="D22" s="86"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+    </row>
+    <row r="23" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="88" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="86" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="86"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="79" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="71" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="85" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="85"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="B12:B22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Fix bugs: booking (allday)
</commit_message>
<xml_diff>
--- a/VacationTracking/Vacation Tracking - Features Estimation.xlsx
+++ b/VacationTracking/Vacation Tracking - Features Estimation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="169">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -1572,6 +1572,51 @@
   <si>
     <t>In week, in month, configurable</t>
   </si>
+  <si>
+    <t>List day off grouped by month</t>
+  </si>
+  <si>
+    <t>Fillter by employee</t>
+  </si>
+  <si>
+    <t>Remaining days off</t>
+  </si>
+  <si>
+    <t>Booking data is invalid. 
+Working Time: 09:00 -&gt; 19:00</t>
+  </si>
+  <si>
+    <t>Booking data is invalid. 
+Lunch Break: 11:30 -&gt; 13:30</t>
+  </si>
+  <si>
+    <t>Configure (working time, lunch break) in appsettings</t>
+  </si>
+  <si>
+    <t>Booking is conflict</t>
+  </si>
+  <si>
+    <t>The remaining vacation day is not enough to booking</t>
+  </si>
+  <si>
+    <t>Vacation duration &gt; {0} days, you do not allow to book within a month</t>
+  </si>
+  <si>
+    <t>Vacation duration &gt; {0} days, you do not allow to book within a week</t>
+  </si>
+  <si>
+    <t>Create
+Update</t>
+  </si>
+  <si>
+    <t>Add/Update booking success</t>
+  </si>
+  <si>
+    <t>Add to top table, remaining day will be reduce accordingly</t>
+  </si>
+  <si>
+    <t>Remove at table, remaining day will be reduce accordingly</t>
+  </si>
 </sst>
 </file>
 
@@ -1822,7 +1867,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2022,10 +2067,12 @@
     <xf numFmtId="0" fontId="19" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2039,6 +2086,24 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2547,7 +2612,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -30874,19 +30939,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="69"/>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -30919,7 +30984,7 @@
       <c r="B3" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="96" t="s">
         <v>49</v>
       </c>
       <c r="D3" s="79" t="s">
@@ -30934,7 +30999,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="82"/>
-      <c r="C4" s="80"/>
+      <c r="C4" s="97"/>
       <c r="D4" s="79" t="s">
         <v>112</v>
       </c>
@@ -30962,7 +31027,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="82"/>
-      <c r="C6" s="79" t="s">
+      <c r="C6" s="96" t="s">
         <v>117</v>
       </c>
       <c r="D6" s="79" t="s">
@@ -30979,7 +31044,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="82"/>
-      <c r="C7" s="80"/>
+      <c r="C7" s="97"/>
       <c r="D7" s="79" t="s">
         <v>112</v>
       </c>
@@ -30992,7 +31057,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="82"/>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="96" t="s">
         <v>122</v>
       </c>
       <c r="D8" s="79" t="s">
@@ -31009,7 +31074,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="82"/>
-      <c r="C9" s="80"/>
+      <c r="C9" s="97"/>
       <c r="D9" s="79" t="s">
         <v>112</v>
       </c>
@@ -31024,7 +31089,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="82"/>
-      <c r="C10" s="79" t="s">
+      <c r="C10" s="96" t="s">
         <v>126</v>
       </c>
       <c r="D10" s="79" t="s">
@@ -31041,7 +31106,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="83"/>
-      <c r="C11" s="80"/>
+      <c r="C11" s="97"/>
       <c r="D11" s="79" t="s">
         <v>112</v>
       </c>
@@ -31056,13 +31121,13 @@
       <c r="B12" s="90" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="79" t="s">
+      <c r="C12" s="96" t="s">
         <v>131</v>
       </c>
-      <c r="D12" s="86" t="s">
+      <c r="D12" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="86" t="s">
+      <c r="E12" s="85" t="s">
         <v>138</v>
       </c>
       <c r="F12" s="80"/>
@@ -31075,11 +31140,11 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="91"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="86" t="s">
+      <c r="C13" s="97"/>
+      <c r="D13" s="85" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="87" t="s">
+      <c r="E13" s="86" t="s">
         <v>135</v>
       </c>
       <c r="F13" s="80"/>
@@ -31088,10 +31153,10 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="91"/>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="85" t="s">
         <v>132</v>
       </c>
-      <c r="D14" s="86" t="s">
+      <c r="D14" s="85" t="s">
         <v>111</v>
       </c>
       <c r="E14" s="80"/>
@@ -31103,10 +31168,10 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="91"/>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="85" t="s">
         <v>133</v>
       </c>
-      <c r="D15" s="86" t="s">
+      <c r="D15" s="85" t="s">
         <v>111</v>
       </c>
       <c r="E15" s="79" t="s">
@@ -31120,10 +31185,10 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="91"/>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="85" t="s">
         <v>134</v>
       </c>
-      <c r="D16" s="86" t="s">
+      <c r="D16" s="85" t="s">
         <v>111</v>
       </c>
       <c r="E16" s="79" t="s">
@@ -31133,36 +31198,42 @@
       <c r="G16" s="80"/>
       <c r="H16" s="80"/>
     </row>
-    <row r="17" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="91"/>
-      <c r="C17" s="86" t="s">
+      <c r="C17" s="85" t="s">
         <v>152</v>
       </c>
-      <c r="D17" s="86"/>
+      <c r="D17" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="E17" s="79"/>
       <c r="F17" s="80"/>
       <c r="G17" s="80"/>
-      <c r="H17" s="86" t="s">
+      <c r="H17" s="85" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="91"/>
-      <c r="C18" s="86" t="s">
+      <c r="C18" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="D18" s="86"/>
+      <c r="D18" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="E18" s="79"/>
       <c r="F18" s="80"/>
       <c r="G18" s="80"/>
       <c r="H18" s="89"/>
     </row>
-    <row r="19" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="91"/>
-      <c r="C19" s="86" t="s">
+      <c r="C19" s="85" t="s">
         <v>149</v>
       </c>
-      <c r="D19" s="86"/>
+      <c r="D19" s="85" t="s">
+        <v>111</v>
+      </c>
       <c r="E19" s="79"/>
       <c r="F19" s="80"/>
       <c r="G19" s="80"/>
@@ -31170,23 +31241,23 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="91"/>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="D20" s="86"/>
+      <c r="D20" s="85"/>
       <c r="E20" s="79"/>
       <c r="F20" s="80"/>
       <c r="G20" s="80"/>
       <c r="H20" s="80"/>
     </row>
-    <row r="21" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="91"/>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="85" t="s">
         <v>144</v>
       </c>
-      <c r="D21" s="86"/>
+      <c r="D21" s="85"/>
       <c r="E21" s="79"/>
       <c r="F21" s="80"/>
       <c r="G21" s="80"/>
@@ -31194,25 +31265,25 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="92"/>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="85" t="s">
         <v>146</v>
       </c>
-      <c r="D22" s="86"/>
+      <c r="D22" s="85"/>
       <c r="E22" s="79"/>
       <c r="F22" s="80"/>
       <c r="G22" s="80"/>
       <c r="H22" s="80"/>
     </row>
-    <row r="23" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="88" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="85" t="s">
         <v>153</v>
       </c>
-      <c r="D23" s="86"/>
+      <c r="D23" s="85"/>
       <c r="E23" s="79"/>
       <c r="F23" s="80"/>
       <c r="G23" s="80"/>
@@ -31220,23 +31291,192 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="71" t="s">
+    <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="71"/>
+      <c r="B24" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="85" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="87"/>
+      <c r="C25" s="85" t="s">
+        <v>156</v>
+      </c>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="80"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="87"/>
+      <c r="C26" s="85" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="80"/>
+      <c r="H26" s="80"/>
+    </row>
+    <row r="27" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B27" s="87" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="85" t="s">
-        <v>38</v>
+      <c r="C27" s="98" t="s">
+        <v>165</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="85"/>
+      <c r="D27" s="79" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="79" t="s">
+        <v>166</v>
+      </c>
+      <c r="F27" s="80"/>
+      <c r="G27" s="79" t="s">
+        <v>137</v>
+      </c>
+      <c r="H27" s="86" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B28" s="87"/>
+      <c r="C28" s="94"/>
+      <c r="D28" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="86" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" s="80"/>
+      <c r="G28" s="80"/>
+      <c r="H28" s="80"/>
+    </row>
+    <row r="29" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B29" s="87"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="86" t="s">
+        <v>159</v>
+      </c>
+      <c r="F29" s="80"/>
+      <c r="G29" s="80"/>
+      <c r="H29" s="80"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="87"/>
+      <c r="C30" s="94"/>
+      <c r="D30" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="79" t="s">
+        <v>161</v>
+      </c>
+      <c r="F30" s="80"/>
+      <c r="G30" s="80"/>
+      <c r="H30" s="80"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="87"/>
+      <c r="C31" s="94"/>
+      <c r="D31" s="85" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" s="85" t="s">
+        <v>162</v>
+      </c>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="80"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="87"/>
+      <c r="C32" s="94"/>
+      <c r="D32" s="85" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" s="85" t="s">
+        <v>163</v>
+      </c>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="87"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="85" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" s="80" t="s">
+        <v>164</v>
+      </c>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="80"/>
+    </row>
+    <row r="34" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B34" s="87"/>
+      <c r="C34" s="79" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" s="79" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="79" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="86" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="87"/>
+      <c r="C35" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="D35" s="79"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="79"/>
+    </row>
+    <row r="36" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B36" s="87"/>
+      <c r="C36" s="93" t="s">
+        <v>160</v>
+      </c>
+      <c r="D36" s="80"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="80"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="10">
+    <mergeCell ref="C27:C33"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
     <mergeCell ref="B3:B11"/>
     <mergeCell ref="B12:B22"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>